<commit_message>
reverse commit bug fixes
</commit_message>
<xml_diff>
--- a/Useful Programs/Matlab/SE_Economy.xlsx
+++ b/Useful Programs/Matlab/SE_Economy.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="209">
   <si>
     <t>Ore</t>
   </si>
@@ -494,9 +494,6 @@
     <t>SubtypeName</t>
   </si>
   <si>
-    <t>Gas</t>
-  </si>
-  <si>
     <t>Modded Items</t>
   </si>
   <si>
@@ -579,21 +576,6 @@
   </si>
   <si>
     <t>HydrogenBottle</t>
-  </si>
-  <si>
-    <t>Oxygen</t>
-  </si>
-  <si>
-    <t>Hydrogen</t>
-  </si>
-  <si>
-    <t>JumpDriveDisruptionMagazine</t>
-  </si>
-  <si>
-    <t>Tribble</t>
-  </si>
-  <si>
-    <t>ShieldComponent</t>
   </si>
   <si>
     <t>StoneOre</t>
@@ -1028,8 +1010,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="D1:N72" totalsRowShown="0" headerRowBorderDxfId="22">
-  <autoFilter ref="D1:N72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="D1:N67" totalsRowShown="0" headerRowBorderDxfId="22">
+  <autoFilter ref="D1:N67"/>
   <tableColumns count="11">
     <tableColumn id="1" name="Unit"/>
     <tableColumn id="11" name="SubtypeName" dataDxfId="21"/>
@@ -1349,7 +1331,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4267,21 +4249,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C38:J38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C20:J20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="C38:J38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="I39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4290,11 +4272,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:W72"/>
+  <dimension ref="C1:W67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F71" sqref="F71"/>
+      <selection pane="bottomLeft" activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4352,7 +4334,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F2" s="11">
         <f>'O&amp;I'!H16</f>
@@ -4397,7 +4379,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="F3" s="11">
         <f>'O&amp;I'!H17</f>
@@ -4442,7 +4424,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F4" s="11">
         <f>'O&amp;I'!H18</f>
@@ -4492,7 +4474,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="F5" s="11">
         <f>'O&amp;I'!H19</f>
@@ -4542,7 +4524,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F6" s="11">
         <f>'O&amp;I'!H20</f>
@@ -4592,7 +4574,7 @@
         <v>9</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="F7" s="11">
         <f>'O&amp;I'!H21</f>
@@ -4642,7 +4624,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F8" s="11">
         <f>'O&amp;I'!H22</f>
@@ -4692,7 +4674,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F9" s="11">
         <f>'O&amp;I'!H23</f>
@@ -4742,7 +4724,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="F10" s="11">
         <f>'O&amp;I'!H24</f>
@@ -4792,7 +4774,7 @@
         <v>13</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="F11" s="11">
         <f>'O&amp;I'!H25</f>
@@ -4894,7 +4876,7 @@
         <v>72</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F13" s="11">
         <f>'O&amp;I'!G16</f>
@@ -4944,7 +4926,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F14" s="11">
         <f>'O&amp;I'!G17</f>
@@ -4994,7 +4976,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F15" s="11">
         <f>'O&amp;I'!G18</f>
@@ -5044,7 +5026,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="F16" s="11">
         <f>'O&amp;I'!G19</f>
@@ -5094,7 +5076,7 @@
         <v>8</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="F17" s="11">
         <f>'O&amp;I'!G20</f>
@@ -5144,7 +5126,7 @@
         <v>9</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F18" s="11">
         <f>'O&amp;I'!G21</f>
@@ -5194,7 +5176,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="F19" s="11">
         <f>'O&amp;I'!G22</f>
@@ -5244,7 +5226,7 @@
         <v>11</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F20" s="11">
         <f>'O&amp;I'!G23</f>
@@ -5294,7 +5276,7 @@
         <v>12</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="F21" s="11">
         <f>'O&amp;I'!G24</f>
@@ -5344,7 +5326,7 @@
         <v>13</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F22" s="11">
         <f>'O&amp;I'!G25</f>
@@ -5391,7 +5373,7 @@
         <v>75</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F23" s="11">
         <f>'Comp. Breakdown'!Y3</f>
@@ -5436,7 +5418,7 @@
         <v>76</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="F24" s="11">
         <f>'Comp. Breakdown'!Y4</f>
@@ -5481,7 +5463,7 @@
         <v>77</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="F25" s="11">
         <f>'Comp. Breakdown'!Y5</f>
@@ -5526,7 +5508,7 @@
         <v>78</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="F26" s="11">
         <f>'Comp. Breakdown'!Y6</f>
@@ -5571,7 +5553,7 @@
         <v>79</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="F27" s="11">
         <f>'Comp. Breakdown'!Y7</f>
@@ -5708,7 +5690,7 @@
         <v>83</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="F30" s="11">
         <f>'Comp. Breakdown'!Y10</f>
@@ -5753,7 +5735,7 @@
         <v>84</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="F31" s="11">
         <f>'Comp. Breakdown'!Y11</f>
@@ -5890,7 +5872,7 @@
         <v>87</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F34" s="11">
         <f>'Comp. Breakdown'!Y14</f>
@@ -5935,7 +5917,7 @@
         <v>88</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="F35" s="11">
         <f>'Comp. Breakdown'!Y15</f>
@@ -5980,7 +5962,7 @@
         <v>89</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="F36" s="11">
         <f>'Comp. Breakdown'!Y16</f>
@@ -6025,7 +6007,7 @@
         <v>90</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F37" s="11">
         <f>'Comp. Breakdown'!Y17</f>
@@ -6072,7 +6054,7 @@
         <v>92</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F38" s="11">
         <f>'Comp. Breakdown'!Y18</f>
@@ -6117,7 +6099,7 @@
         <v>93</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F39" s="11">
         <f>'Comp. Breakdown'!Y19</f>
@@ -6162,7 +6144,7 @@
         <v>94</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F40" s="11">
         <f>'Comp. Breakdown'!Y20</f>
@@ -6207,7 +6189,7 @@
         <v>95</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F41" s="11">
         <f>'Comp. Breakdown'!Y21</f>
@@ -6252,7 +6234,7 @@
         <v>96</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F42" s="11">
         <f>'Comp. Breakdown'!Y22</f>
@@ -6344,7 +6326,7 @@
         <v>99</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F44" s="11">
         <f>'Comp. Breakdown'!Y24</f>
@@ -6391,7 +6373,7 @@
         <v>100</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F45" s="11">
         <f>'Comp. Breakdown'!Y25</f>
@@ -6436,7 +6418,7 @@
         <v>101</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F46" s="11">
         <f>'Comp. Breakdown'!Y26</f>
@@ -6481,7 +6463,7 @@
         <v>102</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F47" s="11">
         <f>'Comp. Breakdown'!Y27</f>
@@ -6528,7 +6510,7 @@
         <v>104</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F48" s="11">
         <f>'Comp. Breakdown'!Y28</f>
@@ -6573,7 +6555,7 @@
         <v>103</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F49" s="11">
         <f>'Comp. Breakdown'!Y29</f>
@@ -6618,7 +6600,7 @@
         <v>105</v>
       </c>
       <c r="E50" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F50" s="11">
         <f>'Comp. Breakdown'!Y30</f>
@@ -6663,7 +6645,7 @@
         <v>106</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F51" s="11">
         <f>'Comp. Breakdown'!Y31</f>
@@ -6708,7 +6690,7 @@
         <v>107</v>
       </c>
       <c r="E52" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F52" s="11">
         <f>'Comp. Breakdown'!Y32</f>
@@ -6753,7 +6735,7 @@
         <v>108</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F53" s="11">
         <f>'Comp. Breakdown'!Y33</f>
@@ -6798,7 +6780,7 @@
         <v>109</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F54" s="11">
         <f>'Comp. Breakdown'!Y34</f>
@@ -6843,7 +6825,7 @@
         <v>110</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F55" s="11">
         <f>'Comp. Breakdown'!Y35</f>
@@ -6888,7 +6870,7 @@
         <v>111</v>
       </c>
       <c r="E56" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F56" s="11">
         <f>'Comp. Breakdown'!Y36</f>
@@ -6933,7 +6915,7 @@
         <v>112</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F57" s="11">
         <f>'Comp. Breakdown'!Y37</f>
@@ -6978,7 +6960,7 @@
         <v>113</v>
       </c>
       <c r="E58" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F58" s="11">
         <f>'Comp. Breakdown'!Y38</f>
@@ -7023,7 +7005,7 @@
         <v>114</v>
       </c>
       <c r="E59" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F59" s="11">
         <f>'Comp. Breakdown'!Y39</f>
@@ -7070,7 +7052,7 @@
         <v>122</v>
       </c>
       <c r="E60" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F60" s="11">
         <f>'Comp. Breakdown'!Y40</f>
@@ -7115,7 +7097,7 @@
         <v>121</v>
       </c>
       <c r="E61" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F61" s="11">
         <f>'Comp. Breakdown'!Y41</f>
@@ -7160,7 +7142,7 @@
         <v>120</v>
       </c>
       <c r="E62" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F62" s="11">
         <f>'Comp. Breakdown'!Y42</f>
@@ -7205,7 +7187,7 @@
         <v>119</v>
       </c>
       <c r="E63" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F63" s="11">
         <f>'Comp. Breakdown'!Y43</f>
@@ -7252,7 +7234,7 @@
         <v>118</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F64" s="11">
         <f>'Comp. Breakdown'!Y44</f>
@@ -7297,7 +7279,7 @@
         <v>117</v>
       </c>
       <c r="E65" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F65" s="11">
         <f>'Comp. Breakdown'!Y45</f>
@@ -7340,24 +7322,40 @@
       <c r="C66" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="E66" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="11"/>
-      <c r="K66" s="11"/>
-      <c r="L66" s="11"/>
-      <c r="M66" s="11"/>
-      <c r="N66" s="11"/>
+      <c r="E66" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="F66" s="11">
+        <v>1</v>
+      </c>
+      <c r="G66" s="11">
+        <v>1</v>
+      </c>
+      <c r="H66" s="11">
+        <v>1</v>
+      </c>
+      <c r="I66" s="11">
+        <v>1</v>
+      </c>
+      <c r="J66" s="11">
+        <v>1</v>
+      </c>
+      <c r="K66" s="11">
+        <v>1</v>
+      </c>
+      <c r="L66" s="11">
+        <v>1</v>
+      </c>
+      <c r="M66" s="11">
+        <v>1</v>
+      </c>
+      <c r="N66" s="11">
+        <v>1</v>
+      </c>
     </row>
     <row r="67" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C67" s="24"/>
-      <c r="E67" s="20" t="s">
-        <v>179</v>
-      </c>
+      <c r="E67" s="20"/>
       <c r="F67" s="11"/>
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
@@ -7368,101 +7366,9 @@
       <c r="M67" s="11"/>
       <c r="N67" s="11"/>
     </row>
-    <row r="68" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C68" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="E68" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="11"/>
-      <c r="K68" s="11"/>
-      <c r="L68" s="11"/>
-      <c r="M68" s="11"/>
-      <c r="N68" s="11"/>
-    </row>
-    <row r="69" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C69" s="24"/>
-      <c r="E69" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="11"/>
-      <c r="K69" s="11"/>
-      <c r="L69" s="11"/>
-      <c r="M69" s="11"/>
-      <c r="N69" s="11"/>
-    </row>
-    <row r="70" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C70" s="24"/>
-      <c r="E70" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="11"/>
-      <c r="J70" s="11"/>
-      <c r="K70" s="11"/>
-      <c r="L70" s="11"/>
-      <c r="M70" s="11"/>
-      <c r="N70" s="11"/>
-    </row>
-    <row r="71" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E71" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="F71" s="11">
-        <v>1</v>
-      </c>
-      <c r="G71" s="11">
-        <v>1</v>
-      </c>
-      <c r="H71" s="11">
-        <v>1</v>
-      </c>
-      <c r="I71" s="11">
-        <v>1</v>
-      </c>
-      <c r="J71" s="11">
-        <v>1</v>
-      </c>
-      <c r="K71" s="11">
-        <v>1</v>
-      </c>
-      <c r="L71" s="11">
-        <v>1</v>
-      </c>
-      <c r="M71" s="11">
-        <v>1</v>
-      </c>
-      <c r="N71" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="E72" s="22"/>
-      <c r="F72" s="11"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="11"/>
-      <c r="I72" s="11"/>
-      <c r="J72" s="11"/>
-      <c r="K72" s="11"/>
-      <c r="L72" s="11"/>
-      <c r="M72" s="11"/>
-      <c r="N72" s="11"/>
-    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="12">
     <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C68:C70"/>
     <mergeCell ref="C38:C42"/>
     <mergeCell ref="C2:C12"/>
     <mergeCell ref="C13:C22"/>

</xml_diff>